<commit_message>
67763 Sprint1 Amend - Review phase in scrum board must have effort attributed to it in burndown (they count as part of the task)
</commit_message>
<xml_diff>
--- a/SE202526/Management/Sprint1/burndown/Sprint1_Burndown.xlsx
+++ b/SE202526/Management/Sprint1/burndown/Sprint1_Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/059c692484dd0481/uni/Semestre5/ES/SE2526_67775_67804_67286_68130_68547_67763/SE202526/Management/Sprint1/burndown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="11_494F38B3C451EBB0AC99F8F5CB09FE5088EA3DC6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94A391E5-F3CA-4A00-9756-1763D378827B}"/>
+  <xr:revisionPtr revIDLastSave="199" documentId="11_494F38B3C451EBB0AC99F8F5CB09FE5088EA3DC6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDF42A53-C033-4929-A318-EFCB9DC234C1}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9855" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="0" windowWidth="12312" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -1155,22 +1155,22 @@
                   <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.4</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.4</c:v>
+                  <c:v>2.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.4</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -1310,25 +1310,25 @@
                   <c:v>9.7000000000000011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.3000000000000007</c:v>
+                  <c:v>9.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.8000000000000007</c:v>
+                  <c:v>7.6000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>5.0000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>4.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.5</c:v>
+                  <c:v>3.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.5</c:v>
+                  <c:v>3.5000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.5</c:v>
+                  <c:v>3.5000000000000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2094,9 +2094,11 @@
         <v>0.2</v>
       </c>
       <c r="J8" s="37">
-        <v>0.2</v>
-      </c>
-      <c r="K8" s="14"/>
+        <v>0.1</v>
+      </c>
+      <c r="K8" s="14">
+        <v>0.1</v>
+      </c>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
       <c r="N8" s="43"/>
@@ -2120,9 +2122,11 @@
       <c r="I9" s="31"/>
       <c r="J9" s="37"/>
       <c r="K9" s="14">
-        <v>1</v>
-      </c>
-      <c r="L9" s="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="L9" s="14">
+        <v>0.5</v>
+      </c>
       <c r="M9" s="14"/>
       <c r="N9" s="43"/>
       <c r="O9" s="37"/>
@@ -2145,14 +2149,16 @@
       <c r="I10" s="31"/>
       <c r="J10" s="37"/>
       <c r="K10" s="14">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
       <c r="N10" s="43">
         <v>0.5</v>
       </c>
-      <c r="O10" s="37"/>
+      <c r="O10" s="37">
+        <v>0.3</v>
+      </c>
       <c r="P10" s="15"/>
     </row>
     <row r="11" spans="2:18" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2175,9 +2181,11 @@
         <v>1</v>
       </c>
       <c r="L11" s="14">
-        <v>1</v>
-      </c>
-      <c r="M11" s="14"/>
+        <v>0.7</v>
+      </c>
+      <c r="M11" s="14">
+        <v>0.3</v>
+      </c>
       <c r="N11" s="43"/>
       <c r="O11" s="37"/>
       <c r="P11" s="15"/>
@@ -2191,51 +2199,51 @@
         <v>0</v>
       </c>
       <c r="E12" s="19">
-        <f>SUM(E6:E11)</f>
+        <f t="shared" ref="E12:P12" si="0">SUM(E6:E11)</f>
         <v>0</v>
       </c>
       <c r="F12" s="20">
-        <f>SUM(F6:F11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G12" s="20">
-        <f>SUM(G6:G11)</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="H12" s="20">
-        <f>SUM(H6:H11)</f>
+        <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
       <c r="I12" s="34">
-        <f>SUM(I6:I11)</f>
+        <f t="shared" si="0"/>
         <v>1.7</v>
       </c>
       <c r="J12" s="38">
-        <f>SUM(J6:J11)</f>
-        <v>0.4</v>
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="K12" s="20">
-        <f>SUM(K6:K11)</f>
-        <v>2.5</v>
+        <f t="shared" si="0"/>
+        <v>1.8</v>
       </c>
       <c r="L12" s="20">
         <f>SUM(L6:L11)</f>
-        <v>2.4</v>
+        <v>2.5999999999999996</v>
       </c>
       <c r="M12" s="20">
-        <f>SUM(M6:M11)</f>
-        <v>0.4</v>
+        <f t="shared" si="0"/>
+        <v>0.7</v>
       </c>
       <c r="N12" s="45">
-        <f>SUM(N6:N11)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="O12" s="20">
-        <f>SUM(O6:O11)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.3</v>
       </c>
       <c r="P12" s="21">
-        <f>SUM(P6:P11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2249,52 +2257,52 @@
         <v>14</v>
       </c>
       <c r="E13" s="23">
-        <f>D13-SUM(E6:E11)</f>
+        <f t="shared" ref="E13:P13" si="1">D13-SUM(E6:E11)</f>
         <v>14</v>
       </c>
       <c r="F13" s="24">
-        <f>E13-SUM(F6:F11)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="G13" s="24">
-        <f>F13-SUM(G6:G11)</f>
+        <f t="shared" si="1"/>
         <v>12.8</v>
       </c>
       <c r="H13" s="24">
-        <f>G13-SUM(H6:H11)</f>
+        <f t="shared" si="1"/>
         <v>11.4</v>
       </c>
       <c r="I13" s="35">
-        <f>H13-SUM(I6:I11)</f>
+        <f t="shared" si="1"/>
         <v>9.7000000000000011</v>
       </c>
       <c r="J13" s="39">
-        <f>I13-SUM(J6:J11)</f>
-        <v>9.3000000000000007</v>
+        <f t="shared" si="1"/>
+        <v>9.4</v>
       </c>
       <c r="K13" s="26">
-        <f>J13-SUM(K6:K11)</f>
-        <v>6.8000000000000007</v>
+        <f t="shared" si="1"/>
+        <v>7.6000000000000005</v>
       </c>
       <c r="L13" s="26">
-        <f>K13-SUM(L6:L11)</f>
-        <v>4.4000000000000004</v>
+        <f t="shared" si="1"/>
+        <v>5.0000000000000009</v>
       </c>
       <c r="M13" s="26">
-        <f>L13-SUM(M6:M11)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>4.3000000000000007</v>
       </c>
       <c r="N13" s="46">
-        <f>M13-SUM(N6:N11)</f>
-        <v>3.5</v>
+        <f t="shared" si="1"/>
+        <v>3.8000000000000007</v>
       </c>
       <c r="O13" s="44">
-        <f>N13-SUM(O6:O11)</f>
-        <v>3.5</v>
+        <f t="shared" si="1"/>
+        <v>3.5000000000000009</v>
       </c>
       <c r="P13" s="25">
-        <f>O13-SUM(P6:P11)</f>
-        <v>3.5</v>
+        <f t="shared" si="1"/>
+        <v>3.5000000000000009</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>